<commit_message>
update structure of excel
</commit_message>
<xml_diff>
--- a/PMD/Output/CreateEmployeeAPI.xlsx
+++ b/PMD/Output/CreateEmployeeAPI.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
   <si>
     <t>SR NUMBER</t>
   </si>
@@ -40,20 +40,22 @@
     <t>ENVIRONMENT</t>
   </si>
   <si>
+    <t>VERSION</t>
+  </si>
+  <si>
     <t>leorek</t>
   </si>
   <si>
     <t>FALSE</t>
   </si>
   <si>
-    <t>801</t>
+    <t>967</t>
   </si>
   <si>
     <t>200</t>
   </si>
   <si>
-    <t xml:space="preserve">
-</t>
+    <t>null</t>
   </si>
   <si>
     <t xml:space="preserve">System.Data.Entity.Core.EntityCommandExecutionException: An error occurred while executing the command definition. See the inner exception for details. ---&gt; Oracle.ManagedDataAccess.Client.OracleException: ORA-00904: "Extent3"."CTURG_ORDRE" : identificateur non valide
@@ -81,96 +83,102 @@
 </t>
   </si>
   <si>
-    <t/>
+    <t>klif</t>
+  </si>
+  <si>
+    <t>v2</t>
   </si>
   <si>
     <t>Antku</t>
   </si>
   <si>
+    <t>234</t>
+  </si>
+  <si>
+    <t>PPLjkiu</t>
+  </si>
+  <si>
+    <t>222</t>
+  </si>
+  <si>
+    <t>chang</t>
+  </si>
+  <si>
+    <t>230</t>
+  </si>
+  <si>
+    <t>Jangri</t>
+  </si>
+  <si>
+    <t>238</t>
+  </si>
+  <si>
+    <t>tappu</t>
+  </si>
+  <si>
+    <t>231</t>
+  </si>
+  <si>
+    <t>ktriya</t>
+  </si>
+  <si>
+    <t>213</t>
+  </si>
+  <si>
+    <t>ANtriya</t>
+  </si>
+  <si>
+    <t>221</t>
+  </si>
+  <si>
+    <t>TeerKn</t>
+  </si>
+  <si>
+    <t>208</t>
+  </si>
+  <si>
+    <t>tappu8</t>
+  </si>
+  <si>
+    <t>219</t>
+  </si>
+  <si>
+    <t>JKS</t>
+  </si>
+  <si>
+    <t>233</t>
+  </si>
+  <si>
+    <t>Antukru</t>
+  </si>
+  <si>
+    <t>Bujiya</t>
+  </si>
+  <si>
+    <t>201</t>
+  </si>
+  <si>
+    <t>tink8k</t>
+  </si>
+  <si>
+    <t>duplicate</t>
+  </si>
+  <si>
     <t>226</t>
   </si>
   <si>
-    <t>PPLjkiu</t>
-  </si>
-  <si>
-    <t>225</t>
-  </si>
-  <si>
-    <t>chang</t>
-  </si>
-  <si>
-    <t>227</t>
-  </si>
-  <si>
-    <t>Jangri</t>
-  </si>
-  <si>
-    <t>254</t>
-  </si>
-  <si>
-    <t>tappu</t>
-  </si>
-  <si>
-    <t>682</t>
-  </si>
-  <si>
-    <t>ktriya</t>
-  </si>
-  <si>
-    <t>224</t>
-  </si>
-  <si>
-    <t>ANtriya</t>
-  </si>
-  <si>
-    <t>214</t>
-  </si>
-  <si>
-    <t>TeerKn</t>
+    <t>luckky</t>
+  </si>
+  <si>
+    <t>223</t>
+  </si>
+  <si>
+    <t>Anmolll</t>
   </si>
   <si>
     <t>216</t>
   </si>
   <si>
-    <t>tappu8</t>
-  </si>
-  <si>
-    <t>206</t>
-  </si>
-  <si>
-    <t>JKS</t>
-  </si>
-  <si>
-    <t>215</t>
-  </si>
-  <si>
-    <t>Antukru</t>
-  </si>
-  <si>
-    <t>Bujiya</t>
-  </si>
-  <si>
-    <t>tink8k</t>
-  </si>
-  <si>
-    <t>223</t>
-  </si>
-  <si>
-    <t>duplicate</t>
-  </si>
-  <si>
-    <t>207</t>
-  </si>
-  <si>
-    <t>luckky</t>
-  </si>
-  <si>
-    <t>217</t>
-  </si>
-  <si>
-    <t>Anmolll</t>
-  </si>
-  <si>
     <t>prach</t>
   </si>
   <si>
@@ -183,7 +191,7 @@
     <t>1bvjhfse</t>
   </si>
   <si>
-    <t>219</t>
+    <t>218</t>
   </si>
   <si>
     <t xml:space="preserve">System.Data.Entity.Core.EntityCommandExecutionException: An error occurred while executing the command definition. See the inner exception for details. ---&gt; Oracle.ManagedDataAccess.Client.OracleException: ORA-00904: "Extent3"."CTURG_ORDRE" : identificateur non valide
@@ -598,7 +606,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main">
   <sheetPr/>
-  <dimension ref="A1:O22"/>
+  <dimension ref="A1:Q22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" topLeftCell="A1" zoomScaleNormal="100" zoomScaleSheetLayoutView="60" zoomScale="100" view="normal"/>
   </sheetViews>
@@ -612,6 +620,7 @@
     <col min="11" max="11" width="35" customWidth="1"/>
     <col min="13" max="13" width="35" customWidth="1"/>
     <col min="15" max="15" width="35" customWidth="1"/>
+    <col min="17" max="17" width="35" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="true" s="1">
@@ -639,31 +648,37 @@
       <c r="O1" s="2" t="s">
         <v>7</v>
       </c>
+      <c r="Q1" s="2" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I2" t="s">
-        <v>11</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>12</v>
+        <v>12</v>
+      </c>
+      <c r="K2" t="s">
+        <v>13</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="O2" t="s">
-        <v>14</v>
+        <v>15</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="3">
@@ -671,25 +686,28 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="I3" t="s">
-        <v>11</v>
-      </c>
-      <c r="K3" s="4" t="s">
-        <v>12</v>
+        <v>12</v>
+      </c>
+      <c r="K3" t="s">
+        <v>13</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="O3" t="s">
-        <v>14</v>
+        <v>15</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="4">
@@ -697,25 +715,28 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="I4" t="s">
-        <v>11</v>
-      </c>
-      <c r="K4" s="4" t="s">
-        <v>12</v>
+        <v>12</v>
+      </c>
+      <c r="K4" t="s">
+        <v>13</v>
       </c>
       <c r="M4" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="O4" t="s">
-        <v>14</v>
+        <v>15</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="5">
@@ -723,25 +744,28 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G5" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="I5" t="s">
-        <v>11</v>
-      </c>
-      <c r="K5" s="4" t="s">
-        <v>12</v>
+        <v>12</v>
+      </c>
+      <c r="K5" t="s">
+        <v>13</v>
       </c>
       <c r="M5" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="O5" t="s">
-        <v>14</v>
+        <v>15</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="6">
@@ -749,25 +773,28 @@
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G6" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="I6" t="s">
-        <v>11</v>
-      </c>
-      <c r="K6" s="4" t="s">
-        <v>12</v>
+        <v>12</v>
+      </c>
+      <c r="K6" t="s">
+        <v>13</v>
       </c>
       <c r="M6" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="O6" t="s">
-        <v>14</v>
+        <v>15</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="7">
@@ -775,25 +802,28 @@
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G7" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="I7" t="s">
-        <v>11</v>
-      </c>
-      <c r="K7" s="4" t="s">
-        <v>12</v>
+        <v>12</v>
+      </c>
+      <c r="K7" t="s">
+        <v>13</v>
       </c>
       <c r="M7" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="O7" t="s">
-        <v>14</v>
+        <v>15</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="8">
@@ -801,25 +831,28 @@
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G8" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="I8" t="s">
-        <v>11</v>
-      </c>
-      <c r="K8" s="4" t="s">
-        <v>12</v>
+        <v>12</v>
+      </c>
+      <c r="K8" t="s">
+        <v>13</v>
       </c>
       <c r="M8" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="O8" t="s">
-        <v>14</v>
+        <v>15</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="9">
@@ -827,25 +860,28 @@
         <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G9" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="I9" t="s">
-        <v>11</v>
-      </c>
-      <c r="K9" s="4" t="s">
-        <v>12</v>
+        <v>12</v>
+      </c>
+      <c r="K9" t="s">
+        <v>13</v>
       </c>
       <c r="M9" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="O9" t="s">
-        <v>14</v>
+        <v>15</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="10">
@@ -853,25 +889,28 @@
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G10" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="I10" t="s">
-        <v>11</v>
-      </c>
-      <c r="K10" s="4" t="s">
-        <v>12</v>
+        <v>12</v>
+      </c>
+      <c r="K10" t="s">
+        <v>13</v>
       </c>
       <c r="M10" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="O10" t="s">
-        <v>14</v>
+        <v>15</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="11">
@@ -879,25 +918,28 @@
         <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G11" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="I11" t="s">
-        <v>11</v>
-      </c>
-      <c r="K11" s="4" t="s">
-        <v>12</v>
+        <v>12</v>
+      </c>
+      <c r="K11" t="s">
+        <v>13</v>
       </c>
       <c r="M11" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="O11" t="s">
-        <v>14</v>
+        <v>15</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="12">
@@ -905,25 +947,28 @@
         <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G12" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="I12" t="s">
-        <v>11</v>
-      </c>
-      <c r="K12" s="4" t="s">
-        <v>12</v>
+        <v>12</v>
+      </c>
+      <c r="K12" t="s">
+        <v>13</v>
       </c>
       <c r="M12" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="O12" t="s">
-        <v>14</v>
+        <v>15</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="13">
@@ -931,25 +976,28 @@
         <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G13" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="I13" t="s">
-        <v>11</v>
-      </c>
-      <c r="K13" s="4" t="s">
-        <v>12</v>
+        <v>12</v>
+      </c>
+      <c r="K13" t="s">
+        <v>13</v>
       </c>
       <c r="M13" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="O13" t="s">
-        <v>14</v>
+        <v>15</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="14">
@@ -957,25 +1005,28 @@
         <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G14" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="I14" t="s">
-        <v>11</v>
-      </c>
-      <c r="K14" s="4" t="s">
-        <v>12</v>
+        <v>12</v>
+      </c>
+      <c r="K14" t="s">
+        <v>13</v>
       </c>
       <c r="M14" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="O14" t="s">
-        <v>14</v>
+        <v>15</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="15">
@@ -983,25 +1034,28 @@
         <v>14</v>
       </c>
       <c r="C15" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G15" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="I15" t="s">
-        <v>11</v>
-      </c>
-      <c r="K15" s="4" t="s">
-        <v>12</v>
+        <v>12</v>
+      </c>
+      <c r="K15" t="s">
+        <v>13</v>
       </c>
       <c r="M15" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="O15" t="s">
-        <v>14</v>
+        <v>15</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="16">
@@ -1009,25 +1063,28 @@
         <v>15</v>
       </c>
       <c r="C16" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G16" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="I16" t="s">
-        <v>11</v>
-      </c>
-      <c r="K16" s="4" t="s">
-        <v>12</v>
+        <v>12</v>
+      </c>
+      <c r="K16" t="s">
+        <v>13</v>
       </c>
       <c r="M16" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="O16" t="s">
-        <v>14</v>
+        <v>15</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="17">
@@ -1035,25 +1092,28 @@
         <v>16</v>
       </c>
       <c r="C17" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G17" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="I17" t="s">
-        <v>11</v>
-      </c>
-      <c r="K17" s="4" t="s">
-        <v>12</v>
+        <v>12</v>
+      </c>
+      <c r="K17" t="s">
+        <v>13</v>
       </c>
       <c r="M17" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="O17" t="s">
-        <v>14</v>
+        <v>15</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="18">
@@ -1061,25 +1121,28 @@
         <v>17</v>
       </c>
       <c r="C18" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G18" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="I18" t="s">
-        <v>11</v>
-      </c>
-      <c r="K18" s="4" t="s">
-        <v>12</v>
+        <v>12</v>
+      </c>
+      <c r="K18" t="s">
+        <v>13</v>
       </c>
       <c r="M18" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="O18" t="s">
-        <v>14</v>
+        <v>15</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="19">
@@ -1087,25 +1150,28 @@
         <v>18</v>
       </c>
       <c r="C19" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G19" t="s">
         <v>42</v>
       </c>
       <c r="I19" t="s">
-        <v>11</v>
-      </c>
-      <c r="K19" s="4" t="s">
-        <v>12</v>
+        <v>12</v>
+      </c>
+      <c r="K19" t="s">
+        <v>13</v>
       </c>
       <c r="M19" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="O19" t="s">
-        <v>14</v>
+        <v>15</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="20">
@@ -1113,25 +1179,28 @@
         <v>19</v>
       </c>
       <c r="C20" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G20" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="I20" t="s">
-        <v>11</v>
-      </c>
-      <c r="K20" s="4" t="s">
-        <v>12</v>
+        <v>12</v>
+      </c>
+      <c r="K20" t="s">
+        <v>13</v>
       </c>
       <c r="M20" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="O20" t="s">
-        <v>14</v>
+        <v>15</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="21">
@@ -1139,25 +1208,28 @@
         <v>20</v>
       </c>
       <c r="C21" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G21" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="I21" t="s">
-        <v>11</v>
-      </c>
-      <c r="K21" s="4" t="s">
-        <v>12</v>
+        <v>12</v>
+      </c>
+      <c r="K21" t="s">
+        <v>13</v>
       </c>
       <c r="M21" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="O21" t="s">
-        <v>14</v>
+        <v>15</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="22">
@@ -1165,25 +1237,28 @@
         <v>21</v>
       </c>
       <c r="C22" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G22" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="I22" t="s">
-        <v>11</v>
-      </c>
-      <c r="K22" s="4" t="s">
-        <v>12</v>
+        <v>12</v>
+      </c>
+      <c r="K22" t="s">
+        <v>13</v>
       </c>
       <c r="M22" s="4" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="O22" t="s">
-        <v>14</v>
+        <v>15</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Correct ID for salarycostAPI
</commit_message>
<xml_diff>
--- a/PMD/Output/CreateEmployeeAPI.xlsx
+++ b/PMD/Output/CreateEmployeeAPI.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="59">
   <si>
     <t>SR NUMBER</t>
   </si>
@@ -49,40 +49,20 @@
     <t>FALSE</t>
   </si>
   <si>
-    <t>967</t>
+    <t>17203</t>
   </si>
   <si>
     <t>200</t>
   </si>
   <si>
-    <t>null</t>
-  </si>
-  <si>
-    <t xml:space="preserve">System.Data.Entity.Core.EntityCommandExecutionException: An error occurred while executing the command definition. See the inner exception for details. ---&gt; Oracle.ManagedDataAccess.Client.OracleException: ORA-00904: "Extent3"."CTURG_ORDRE" : identificateur non valide
-   at OracleInternal.ServiceObjects.OracleConnectionImpl.VerifyExecution(Int32&amp; cursorId, Boolean bThrowArrayBindRelatedErrors, SqlStatementType sqlStatementType, Int32 arrayBindCount, OracleException&amp; exceptionForArrayBindDML, Boolean&amp; hasMoreRowsInDB, Boolean bFirstIterationDone)
-   at OracleInternal.ServiceObjects.OracleCommandImpl.ExecuteReader(String commandText, OracleParameterCollection paramColl, CommandType commandType, OracleConnectionImpl connectionImpl, OracleDataReaderImpl&amp; rdrImpl, Int32 longFetchSize, Int64 clientInitialLOBFS, OracleDependencyImpl orclDependencyImpl, Int64[] scnForExecution, Int64[]&amp; scnFromExecution, OracleParameterCollection&amp; bindByPositionParamColl, Boolean&amp; bBindParamPresent, Int64&amp; internalInitialLOBFS, OracleException&amp; exceptionForArrayBindDML, OracleConnection connection, OracleLogicalTransaction&amp; oracleLogicalTransaction, IEnumerable`1 adrianParsedStmt, Boolean isDescribeOnly, Boolean isFromEF)
-   at Oracle.ManagedDataAccess.Client.OracleCommand.ExecuteReader(Boolean requery, Boolean fillRequest, CommandBehavior behavior)
-   at Oracle.ManagedDataAccess.Client.OracleCommand.ExecuteDbDataReader(CommandBehavior behavior)
-   at System.Data.Entity.Infrastructure.Interception.InternalDispatcher`1.Dispatch[TTarget,TInterceptionContext,TResult](TTarget target, Func`3 operation, TInterceptionContext interceptionContext, Action`3 executing, Action`3 executed)
-   at System.Data.Entity.Infrastructure.Interception.DbCommandDispatcher.Reader(DbCommand command, DbCommandInterceptionContext interceptionContext)
-   at System.Data.Entity.Core.EntityClient.Internal.EntityCommandDefinition.ExecuteStoreCommands(EntityCommand entityCommand, CommandBehavior behavior)
-   --- End of inner exception stack trace ---
-   at System.Data.Entity.Core.EntityClient.Internal.EntityCommandDefinition.ExecuteStoreCommands(EntityCommand entityCommand, CommandBehavior behavior)
-   at System.Data.Entity.Core.Objects.Internal.ObjectQueryExecutionPlan.Execute[TResultType](ObjectContext context, ObjectParameterCollection parameterValues)
-   at System.Data.Entity.Core.Objects.ObjectContext.ExecuteInTransaction[T](Func`1 func, IDbExecutionStrategy executionStrategy, Boolean startLocalTransaction, Boolean releaseConnectionOnSuccess)
-   at System.Data.Entity.Core.Objects.ObjectQuery`1.&lt;&gt;c__DisplayClass7.&lt;GetResults&gt;b__5()
-   at System.Data.Entity.Core.Objects.ObjectQuery`1.GetResults(Nullable`1 forMergeOption)
-   at System.Data.Entity.Core.Objects.ObjectQuery`1.&lt;System.Collections.Generic.IEnumerable&lt;T&gt;.GetEnumerator&gt;b__0()
-   at System.Data.Entity.Internal.LazyEnumerator`1.MoveNext()
-   at System.Collections.Generic.List`1..ctor(IEnumerable`1 collection)
-   at System.Linq.Enumerable.ToList[TSource](IEnumerable`1 source)
-   at MVCFramework.Business.Base.Service.AggregationServiceBase`2.Get(Operations operations, Nullable`1 page, Nullable`1 pageSize)
-   at PeopleMasterDataAPI.Services.GlobalEmployee.GlobalEmployeeService.FillIdPersonByNameAndBirthdate(GlobalEmployeeInsertUpdateModel element) in D:\WISAZDOAG02.MVC_Pool\_work\10\s\PeopleMasterDataAPI.Services\Services\GlobalEmployee\GlobalEmployeeService.cs:line 1786
-   at PeopleMasterDataAPI.Services.GlobalEmployee.GlobalEmployeeService.SaveGlobalEmployee(GlobalEmployeeInsertUpdateModel element) in D:\WISAZDOAG02.MVC_Pool\_work\10\s\PeopleMasterDataAPI.Services\Services\GlobalEmployee\GlobalEmployeeService.cs:line 1098
-   at PeopleMasterDataAPI.Web.Controllers.GlobalEmployee.v2.GlobalEmployeeV2Controller.Update(GlobalEmployeeInsertUpdateModel model) in D:\WISAZDOAG02.MVC_Pool\_work\10\s\PeopleMasterDataAPI.Web\Controllers\GlobalEmployee\v2\GlobalEmployeeV2Controller.cs:line 155
+    <t xml:space="preserve">0014
 </t>
   </si>
   <si>
+    <t xml:space="preserve">Impossible to insert a duplicate for this employee.
+</t>
+  </si>
+  <si>
     <t>klif</t>
   </si>
   <si>
@@ -92,131 +72,129 @@
     <t>Antku</t>
   </si>
   <si>
-    <t>234</t>
+    <t>2127</t>
   </si>
   <si>
     <t>PPLjkiu</t>
   </si>
   <si>
-    <t>222</t>
+    <t>2062</t>
   </si>
   <si>
     <t>chang</t>
   </si>
   <si>
-    <t>230</t>
+    <t>2140</t>
   </si>
   <si>
     <t>Jangri</t>
   </si>
   <si>
-    <t>238</t>
+    <t>2189</t>
   </si>
   <si>
     <t>tappu</t>
   </si>
   <si>
-    <t>231</t>
+    <t>2045</t>
   </si>
   <si>
     <t>ktriya</t>
   </si>
   <si>
-    <t>213</t>
+    <t>2321</t>
   </si>
   <si>
     <t>ANtriya</t>
   </si>
   <si>
-    <t>221</t>
+    <t>2073</t>
   </si>
   <si>
     <t>TeerKn</t>
   </si>
   <si>
-    <t>208</t>
+    <t>1993</t>
   </si>
   <si>
     <t>tappu8</t>
   </si>
   <si>
-    <t>219</t>
+    <t>12344</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0041
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A forbidden special character has been included for the field LastName. Please delete it from the field in order to continue.
+</t>
   </si>
   <si>
     <t>JKS</t>
   </si>
   <si>
-    <t>233</t>
+    <t>2292</t>
   </si>
   <si>
     <t>Antukru</t>
   </si>
   <si>
+    <t>2054</t>
+  </si>
+  <si>
     <t>Bujiya</t>
   </si>
   <si>
-    <t>201</t>
+    <t>2311</t>
   </si>
   <si>
     <t>tink8k</t>
   </si>
   <si>
+    <t>4941</t>
+  </si>
+  <si>
     <t>duplicate</t>
   </si>
   <si>
-    <t>226</t>
+    <t>2096</t>
   </si>
   <si>
     <t>luckky</t>
   </si>
   <si>
-    <t>223</t>
+    <t>2192</t>
   </si>
   <si>
     <t>Anmolll</t>
   </si>
   <si>
-    <t>216</t>
+    <t>2253</t>
   </si>
   <si>
     <t>prach</t>
   </si>
   <si>
+    <t>2391</t>
+  </si>
+  <si>
     <t>chipstwiohfwuifwh</t>
   </si>
   <si>
+    <t>2173</t>
+  </si>
+  <si>
     <t>qauartxsd</t>
   </si>
   <si>
+    <t>2008</t>
+  </si>
+  <si>
     <t>1bvjhfse</t>
   </si>
   <si>
-    <t>218</t>
-  </si>
-  <si>
-    <t xml:space="preserve">System.Data.Entity.Core.EntityCommandExecutionException: An error occurred while executing the command definition. See the inner exception for details. ---&gt; Oracle.ManagedDataAccess.Client.OracleException: ORA-00904: "Extent3"."CTURG_ORDRE" : identificateur non valide
-   at OracleInternal.ServiceObjects.OracleConnectionImpl.VerifyExecution(Int32&amp; cursorId, Boolean bThrowArrayBindRelatedErrors, SqlStatementType sqlStatementType, Int32 arrayBindCount, OracleException&amp; exceptionForArrayBindDML, Boolean&amp; hasMoreRowsInDB, Boolean bFirstIterationDone)
-   at OracleInternal.ServiceObjects.OracleCommandImpl.ExecuteReader(String commandText, OracleParameterCollection paramColl, CommandType commandType, OracleConnectionImpl connectionImpl, OracleDataReaderImpl&amp; rdrImpl, Int32 longFetchSize, Int64 clientInitialLOBFS, OracleDependencyImpl orclDependencyImpl, Int64[] scnForExecution, Int64[]&amp; scnFromExecution, OracleParameterCollection&amp; bindByPositionParamColl, Boolean&amp; bBindParamPresent, Int64&amp; internalInitialLOBFS, OracleException&amp; exceptionForArrayBindDML, OracleConnection connection, OracleLogicalTransaction&amp; oracleLogicalTransaction, IEnumerable`1 adrianParsedStmt, Boolean isDescribeOnly, Boolean isFromEF)
-   at Oracle.ManagedDataAccess.Client.OracleCommand.ExecuteReader(Boolean requery, Boolean fillRequest, CommandBehavior behavior)
-   at Oracle.ManagedDataAccess.Client.OracleCommand.ExecuteDbDataReader(CommandBehavior behavior)
-   at System.Data.Entity.Infrastructure.Interception.InternalDispatcher`1.Dispatch[TTarget,TInterceptionContext,TResult](TTarget target, Func`3 operation, TInterceptionContext interceptionContext, Action`3 executing, Action`3 executed)
-   at System.Data.Entity.Infrastructure.Interception.DbCommandDispatcher.Reader(DbCommand command, DbCommandInterceptionContext interceptionContext)
-   at System.Data.Entity.Core.EntityClient.Internal.EntityCommandDefinition.ExecuteStoreCommands(EntityCommand entityCommand, CommandBehavior behavior)
-   --- End of inner exception stack trace ---
-   at System.Data.Entity.Core.EntityClient.Internal.EntityCommandDefinition.ExecuteStoreCommands(EntityCommand entityCommand, CommandBehavior behavior)
-   at System.Data.Entity.Core.Objects.Internal.ObjectQueryExecutionPlan.Execute[TResultType](ObjectContext context, ObjectParameterCollection parameterValues)
-   at System.Data.Entity.Core.Objects.ObjectContext.ExecuteInTransaction[T](Func`1 func, IDbExecutionStrategy executionStrategy, Boolean startLocalTransaction, Boolean releaseConnectionOnSuccess)
-   at System.Data.Entity.Core.Objects.ObjectQuery`1.&lt;&gt;c__DisplayClass7.&lt;GetResults&gt;b__5()
-   at System.Data.Entity.Core.Objects.ObjectQuery`1.GetResults(Nullable`1 forMergeOption)
-   at System.Data.Entity.Core.Objects.ObjectQuery`1.&lt;System.Collections.Generic.IEnumerable&lt;T&gt;.GetEnumerator&gt;b__0()
-   at System.Data.Entity.Internal.LazyEnumerator`1.MoveNext()
-   at System.Collections.Generic.List`1..ctor(IEnumerable`1 collection)
-   at System.Linq.Enumerable.ToList[TSource](IEnumerable`1 source)
-   at MVCFramework.Business.Base.Service.AggregationServiceBase`2.Get(Operations operations, Nullable`1 page, Nullable`1 pageSize)
-   at PeopleMasterDataAPI.Services.GlobalEmployee.GlobalEmployeeService.FillIdPersonByNameAndBirthdate(GlobalEmployeeInsertUpdateModel element) in D:\WISAZDOAG02.MVC_Pool\_work\10\s\PeopleMasterDataAPI.Services\Services\GlobalEmployee\GlobalEmployeeService.cs:line 1786
-   at PeopleMasterDataAPI.Services.GlobalEmployee.GlobalEmployeeService.SaveGlobalEmployee(GlobalEmployeeInsertUpdateModel element) in D:\WISAZDOAG02.MVC_Pool\_work\10\s\PeopleMasterDataAPI.Services\Services\GlobalEmployee\GlobalEmployeeService.cs:line 1098
-   at PeopleMasterDataAPI.Web.Controllers.GlobalEmployee.v2.GlobalEmployeeV2Controller.Update(GlobalEmployeeInsertUpdateModel model) in D:\WISAZDOAG02.MVC_Pool\_work\10\s\PeopleMasterDataAPI.Web\Controllers\GlobalEmployee\v2\GlobalEmployeeV2Controller.cs:line 155
-</t>
+    <t>5215</t>
   </si>
 </sst>
 </file>
@@ -668,7 +646,7 @@
       <c r="I2" t="s">
         <v>12</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K2" s="4" t="s">
         <v>13</v>
       </c>
       <c r="M2" s="4" t="s">
@@ -697,7 +675,7 @@
       <c r="I3" t="s">
         <v>12</v>
       </c>
-      <c r="K3" t="s">
+      <c r="K3" s="4" t="s">
         <v>13</v>
       </c>
       <c r="M3" s="4" t="s">
@@ -726,7 +704,7 @@
       <c r="I4" t="s">
         <v>12</v>
       </c>
-      <c r="K4" t="s">
+      <c r="K4" s="4" t="s">
         <v>13</v>
       </c>
       <c r="M4" s="4" t="s">
@@ -755,7 +733,7 @@
       <c r="I5" t="s">
         <v>12</v>
       </c>
-      <c r="K5" t="s">
+      <c r="K5" s="4" t="s">
         <v>13</v>
       </c>
       <c r="M5" s="4" t="s">
@@ -784,7 +762,7 @@
       <c r="I6" t="s">
         <v>12</v>
       </c>
-      <c r="K6" t="s">
+      <c r="K6" s="4" t="s">
         <v>13</v>
       </c>
       <c r="M6" s="4" t="s">
@@ -813,7 +791,7 @@
       <c r="I7" t="s">
         <v>12</v>
       </c>
-      <c r="K7" t="s">
+      <c r="K7" s="4" t="s">
         <v>13</v>
       </c>
       <c r="M7" s="4" t="s">
@@ -842,7 +820,7 @@
       <c r="I8" t="s">
         <v>12</v>
       </c>
-      <c r="K8" t="s">
+      <c r="K8" s="4" t="s">
         <v>13</v>
       </c>
       <c r="M8" s="4" t="s">
@@ -871,7 +849,7 @@
       <c r="I9" t="s">
         <v>12</v>
       </c>
-      <c r="K9" t="s">
+      <c r="K9" s="4" t="s">
         <v>13</v>
       </c>
       <c r="M9" s="4" t="s">
@@ -900,7 +878,7 @@
       <c r="I10" t="s">
         <v>12</v>
       </c>
-      <c r="K10" t="s">
+      <c r="K10" s="4" t="s">
         <v>13</v>
       </c>
       <c r="M10" s="4" t="s">
@@ -929,11 +907,11 @@
       <c r="I11" t="s">
         <v>12</v>
       </c>
-      <c r="K11" t="s">
-        <v>13</v>
+      <c r="K11" s="4" t="s">
+        <v>35</v>
       </c>
       <c r="M11" s="4" t="s">
-        <v>14</v>
+        <v>36</v>
       </c>
       <c r="O11" t="s">
         <v>15</v>
@@ -947,18 +925,18 @@
         <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>10</v>
       </c>
       <c r="G12" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="I12" t="s">
         <v>12</v>
       </c>
-      <c r="K12" t="s">
+      <c r="K12" s="4" t="s">
         <v>13</v>
       </c>
       <c r="M12" s="4" t="s">
@@ -976,18 +954,18 @@
         <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>10</v>
       </c>
       <c r="G13" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="I13" t="s">
         <v>12</v>
       </c>
-      <c r="K13" t="s">
+      <c r="K13" s="4" t="s">
         <v>13</v>
       </c>
       <c r="M13" s="4" t="s">
@@ -1005,18 +983,18 @@
         <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>10</v>
       </c>
       <c r="G14" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="I14" t="s">
         <v>12</v>
       </c>
-      <c r="K14" t="s">
+      <c r="K14" s="4" t="s">
         <v>13</v>
       </c>
       <c r="M14" s="4" t="s">
@@ -1034,22 +1012,22 @@
         <v>14</v>
       </c>
       <c r="C15" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>10</v>
       </c>
       <c r="G15" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="I15" t="s">
         <v>12</v>
       </c>
-      <c r="K15" t="s">
-        <v>13</v>
+      <c r="K15" s="4" t="s">
+        <v>35</v>
       </c>
       <c r="M15" s="4" t="s">
-        <v>14</v>
+        <v>36</v>
       </c>
       <c r="O15" t="s">
         <v>15</v>
@@ -1063,18 +1041,18 @@
         <v>15</v>
       </c>
       <c r="C16" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>10</v>
       </c>
       <c r="G16" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="I16" t="s">
         <v>12</v>
       </c>
-      <c r="K16" t="s">
+      <c r="K16" s="4" t="s">
         <v>13</v>
       </c>
       <c r="M16" s="4" t="s">
@@ -1092,18 +1070,18 @@
         <v>16</v>
       </c>
       <c r="C17" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>10</v>
       </c>
       <c r="G17" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="I17" t="s">
         <v>12</v>
       </c>
-      <c r="K17" t="s">
+      <c r="K17" s="4" t="s">
         <v>13</v>
       </c>
       <c r="M17" s="4" t="s">
@@ -1121,18 +1099,18 @@
         <v>17</v>
       </c>
       <c r="C18" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="E18" s="3" t="s">
         <v>10</v>
       </c>
       <c r="G18" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="I18" t="s">
         <v>12</v>
       </c>
-      <c r="K18" t="s">
+      <c r="K18" s="4" t="s">
         <v>13</v>
       </c>
       <c r="M18" s="4" t="s">
@@ -1150,18 +1128,18 @@
         <v>18</v>
       </c>
       <c r="C19" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>10</v>
       </c>
       <c r="G19" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="I19" t="s">
         <v>12</v>
       </c>
-      <c r="K19" t="s">
+      <c r="K19" s="4" t="s">
         <v>13</v>
       </c>
       <c r="M19" s="4" t="s">
@@ -1179,18 +1157,18 @@
         <v>19</v>
       </c>
       <c r="C20" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>10</v>
       </c>
       <c r="G20" t="s">
-        <v>28</v>
+        <v>54</v>
       </c>
       <c r="I20" t="s">
         <v>12</v>
       </c>
-      <c r="K20" t="s">
+      <c r="K20" s="4" t="s">
         <v>13</v>
       </c>
       <c r="M20" s="4" t="s">
@@ -1208,18 +1186,18 @@
         <v>20</v>
       </c>
       <c r="C21" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>10</v>
       </c>
       <c r="G21" t="s">
-        <v>18</v>
+        <v>56</v>
       </c>
       <c r="I21" t="s">
         <v>12</v>
       </c>
-      <c r="K21" t="s">
+      <c r="K21" s="4" t="s">
         <v>13</v>
       </c>
       <c r="M21" s="4" t="s">
@@ -1237,22 +1215,22 @@
         <v>21</v>
       </c>
       <c r="C22" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="E22" s="5" t="s">
         <v>10</v>
       </c>
       <c r="G22" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="I22" t="s">
         <v>12</v>
       </c>
-      <c r="K22" t="s">
-        <v>13</v>
+      <c r="K22" s="4" t="s">
+        <v>35</v>
       </c>
       <c r="M22" s="4" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="O22" t="s">
         <v>15</v>

</xml_diff>